<commit_message>
Update HOTAS Switch and Button - Quick Reference - FULL.xlsx
Update for v5.0.0
</commit_message>
<xml_diff>
--- a/Maps/HOTAS Switch and Button - Quick Reference - FULL.xlsx
+++ b/Maps/HOTAS Switch and Button - Quick Reference - FULL.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="424" uniqueCount="222">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="429" uniqueCount="229">
   <si>
     <t>TG1</t>
   </si>
@@ -623,18 +623,9 @@
     <t>Solo</t>
   </si>
   <si>
-    <t>GameLoaded = 0</t>
-  </si>
-  <si>
     <t>Reset Status LEDs</t>
   </si>
   <si>
-    <t>fnDebugStates(DebugON)</t>
-  </si>
-  <si>
-    <t>fnDebugStates(DebugOFF)</t>
-  </si>
-  <si>
     <t>IDLELOFF</t>
   </si>
   <si>
@@ -690,6 +681,36 @@
   </si>
   <si>
     <t>HOTAS - Quick reference - v5.0.0 - FULL</t>
+  </si>
+  <si>
+    <t>fnPrintState()</t>
+  </si>
+  <si>
+    <t>stfnDumpFlags()</t>
+  </si>
+  <si>
+    <t>fnDebug(2)</t>
+  </si>
+  <si>
+    <t>fnDebug(1)</t>
+  </si>
+  <si>
+    <t>fnDebug(3)</t>
+  </si>
+  <si>
+    <t>ShowFlags</t>
+  </si>
+  <si>
+    <t>Debug</t>
+  </si>
+  <si>
+    <t>both</t>
+  </si>
+  <si>
+    <t>IU</t>
+  </si>
+  <si>
+    <t>OM</t>
   </si>
 </sst>
 </file>
@@ -1311,20 +1332,29 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="31" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1334,15 +1364,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1642,7 +1663,7 @@
   <dimension ref="A1:O101"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:O2"/>
+      <selection activeCell="M15" sqref="M15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1667,22 +1688,22 @@
   <sheetData>
     <row r="1" spans="2:15" s="2" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="2:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="58" t="s">
-        <v>221</v>
-      </c>
-      <c r="C2" s="59"/>
-      <c r="D2" s="59"/>
-      <c r="E2" s="59"/>
-      <c r="F2" s="59"/>
-      <c r="G2" s="59"/>
-      <c r="H2" s="59"/>
-      <c r="I2" s="59"/>
-      <c r="J2" s="59"/>
-      <c r="K2" s="59"/>
-      <c r="L2" s="59"/>
-      <c r="M2" s="59"/>
-      <c r="N2" s="59"/>
-      <c r="O2" s="60"/>
+      <c r="B2" s="55" t="s">
+        <v>218</v>
+      </c>
+      <c r="C2" s="56"/>
+      <c r="D2" s="56"/>
+      <c r="E2" s="56"/>
+      <c r="F2" s="56"/>
+      <c r="G2" s="56"/>
+      <c r="H2" s="56"/>
+      <c r="I2" s="56"/>
+      <c r="J2" s="56"/>
+      <c r="K2" s="56"/>
+      <c r="L2" s="56"/>
+      <c r="M2" s="56"/>
+      <c r="N2" s="56"/>
+      <c r="O2" s="57"/>
     </row>
     <row r="3" spans="2:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="4" spans="2:15" x14ac:dyDescent="0.25">
@@ -1693,7 +1714,7 @@
       <c r="D4" s="63"/>
       <c r="E4" s="64"/>
       <c r="G4" s="62" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
       <c r="H4" s="63"/>
       <c r="I4" s="63"/>
@@ -1758,7 +1779,7 @@
       <c r="O6" s="15"/>
     </row>
     <row r="7" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B7" s="50" t="s">
+      <c r="B7" s="53" t="s">
         <v>0</v>
       </c>
       <c r="C7" s="31" t="s">
@@ -1776,7 +1797,7 @@
         <v>115</v>
       </c>
       <c r="J7" s="20"/>
-      <c r="L7" s="50" t="s">
+      <c r="L7" s="53" t="s">
         <v>73</v>
       </c>
       <c r="M7" s="38" t="s">
@@ -1788,7 +1809,7 @@
       <c r="O7" s="39"/>
     </row>
     <row r="8" spans="2:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B8" s="52"/>
+      <c r="B8" s="51"/>
       <c r="C8" s="3" t="s">
         <v>25</v>
       </c>
@@ -1806,7 +1827,7 @@
         <v>116</v>
       </c>
       <c r="J8" s="21"/>
-      <c r="L8" s="51"/>
+      <c r="L8" s="52"/>
       <c r="M8" s="5" t="s">
         <v>128</v>
       </c>
@@ -1816,7 +1837,7 @@
       <c r="O8" s="6"/>
     </row>
     <row r="9" spans="2:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B9" s="51"/>
+      <c r="B9" s="52"/>
       <c r="C9" s="5" t="s">
         <v>26</v>
       </c>
@@ -1824,7 +1845,7 @@
         <v>137</v>
       </c>
       <c r="E9" s="6" t="s">
-        <v>213</v>
+        <v>210</v>
       </c>
       <c r="G9" s="37" t="s">
         <v>113</v>
@@ -1841,7 +1862,7 @@
         <v>25</v>
       </c>
       <c r="N9" s="48" t="s">
-        <v>214</v>
+        <v>211</v>
       </c>
       <c r="O9" s="49"/>
     </row>
@@ -1858,14 +1879,14 @@
       <c r="H10" s="15"/>
       <c r="I10" s="15"/>
       <c r="J10" s="15"/>
-      <c r="L10" s="50" t="s">
+      <c r="L10" s="53" t="s">
         <v>75</v>
       </c>
       <c r="M10" s="38" t="s">
         <v>127</v>
       </c>
       <c r="N10" s="38" t="s">
-        <v>215</v>
+        <v>212</v>
       </c>
       <c r="O10" s="39"/>
     </row>
@@ -1876,7 +1897,7 @@
       </c>
       <c r="D11" s="3"/>
       <c r="E11" s="23"/>
-      <c r="G11" s="55" t="s">
+      <c r="G11" s="58" t="s">
         <v>50</v>
       </c>
       <c r="H11" s="12" t="s">
@@ -1886,23 +1907,23 @@
         <v>52</v>
       </c>
       <c r="J11" s="13"/>
-      <c r="L11" s="51"/>
+      <c r="L11" s="52"/>
       <c r="M11" s="5" t="s">
         <v>128</v>
       </c>
       <c r="N11" s="24" t="s">
-        <v>216</v>
+        <v>213</v>
       </c>
       <c r="O11" s="6"/>
     </row>
     <row r="12" spans="2:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B12" s="51"/>
+      <c r="B12" s="52"/>
       <c r="C12" s="24" t="s">
         <v>26</v>
       </c>
       <c r="D12" s="24"/>
       <c r="E12" s="6"/>
-      <c r="G12" s="56"/>
+      <c r="G12" s="59"/>
       <c r="H12" s="3" t="s">
         <v>25</v>
       </c>
@@ -1920,25 +1941,25 @@
       <c r="C13" s="15"/>
       <c r="D13" s="15"/>
       <c r="E13" s="15"/>
-      <c r="G13" s="57"/>
+      <c r="G13" s="60"/>
       <c r="H13" s="5" t="s">
         <v>26</v>
       </c>
       <c r="I13" s="5"/>
       <c r="J13" s="6"/>
-      <c r="L13" s="50" t="s">
+      <c r="L13" s="53" t="s">
         <v>76</v>
       </c>
       <c r="M13" s="38" t="s">
-        <v>127</v>
+        <v>227</v>
       </c>
       <c r="N13" s="38" t="s">
-        <v>217</v>
+        <v>214</v>
       </c>
       <c r="O13" s="39"/>
     </row>
     <row r="14" spans="2:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B14" s="50" t="s">
+      <c r="B14" s="53" t="s">
         <v>27</v>
       </c>
       <c r="C14" s="12" t="s">
@@ -1952,9 +1973,9 @@
       <c r="H14" s="15"/>
       <c r="I14" s="15"/>
       <c r="J14" s="15"/>
-      <c r="L14" s="51"/>
+      <c r="L14" s="52"/>
       <c r="M14" s="5" t="s">
-        <v>128</v>
+        <v>228</v>
       </c>
       <c r="N14" s="5" t="s">
         <v>176</v>
@@ -1962,7 +1983,7 @@
       <c r="O14" s="6"/>
     </row>
     <row r="15" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B15" s="52"/>
+      <c r="B15" s="51"/>
       <c r="C15" s="3" t="s">
         <v>25</v>
       </c>
@@ -1970,7 +1991,7 @@
         <v>4</v>
       </c>
       <c r="E15" s="4"/>
-      <c r="G15" s="55" t="s">
+      <c r="G15" s="58" t="s">
         <v>53</v>
       </c>
       <c r="H15" s="25" t="s">
@@ -1980,7 +2001,7 @@
         <v>161</v>
       </c>
       <c r="J15" s="26"/>
-      <c r="L15" s="52" t="s">
+      <c r="L15" s="51" t="s">
         <v>77</v>
       </c>
       <c r="M15" s="7"/>
@@ -1988,15 +2009,15 @@
       <c r="O15" s="8"/>
     </row>
     <row r="16" spans="2:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B16" s="51"/>
+      <c r="B16" s="52"/>
       <c r="C16" s="5" t="s">
         <v>26</v>
       </c>
       <c r="D16" s="5" t="s">
-        <v>211</v>
+        <v>208</v>
       </c>
       <c r="E16" s="6"/>
-      <c r="G16" s="56"/>
+      <c r="G16" s="59"/>
       <c r="H16" s="3" t="s">
         <v>25</v>
       </c>
@@ -2004,7 +2025,7 @@
         <v>54</v>
       </c>
       <c r="J16" s="4"/>
-      <c r="L16" s="52"/>
+      <c r="L16" s="51"/>
       <c r="M16" s="3" t="s">
         <v>25</v>
       </c>
@@ -2018,19 +2039,19 @@
       <c r="C17" s="15"/>
       <c r="D17" s="15"/>
       <c r="E17" s="15"/>
-      <c r="G17" s="57"/>
+      <c r="G17" s="60"/>
       <c r="H17" s="5" t="s">
         <v>26</v>
       </c>
       <c r="I17" s="5"/>
       <c r="J17" s="6"/>
-      <c r="L17" s="51"/>
+      <c r="L17" s="52"/>
       <c r="M17" s="5"/>
       <c r="N17" s="5"/>
       <c r="O17" s="6"/>
     </row>
     <row r="18" spans="2:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B18" s="50" t="s">
+      <c r="B18" s="53" t="s">
         <v>108</v>
       </c>
       <c r="C18" s="29" t="s">
@@ -2048,7 +2069,7 @@
       <c r="J18" s="15"/>
     </row>
     <row r="19" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B19" s="52"/>
+      <c r="B19" s="51"/>
       <c r="C19" s="3" t="s">
         <v>25</v>
       </c>
@@ -2058,7 +2079,7 @@
       <c r="E19" s="4" t="s">
         <v>129</v>
       </c>
-      <c r="G19" s="50" t="s">
+      <c r="G19" s="53" t="s">
         <v>55</v>
       </c>
       <c r="H19" s="12" t="s">
@@ -2066,19 +2087,19 @@
       </c>
       <c r="I19" s="12"/>
       <c r="J19" s="13"/>
-      <c r="L19" s="50" t="s">
+      <c r="L19" s="53" t="s">
         <v>78</v>
       </c>
       <c r="M19" s="38" t="s">
         <v>127</v>
       </c>
       <c r="N19" s="38" t="s">
-        <v>218</v>
+        <v>215</v>
       </c>
       <c r="O19" s="39"/>
     </row>
     <row r="20" spans="2:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B20" s="51"/>
+      <c r="B20" s="52"/>
       <c r="C20" s="5" t="s">
         <v>26</v>
       </c>
@@ -2086,9 +2107,9 @@
         <v>138</v>
       </c>
       <c r="E20" s="6" t="s">
-        <v>213</v>
-      </c>
-      <c r="G20" s="52"/>
+        <v>210</v>
+      </c>
+      <c r="G20" s="51"/>
       <c r="H20" s="3" t="s">
         <v>25</v>
       </c>
@@ -2098,7 +2119,7 @@
       <c r="J20" s="4" t="s">
         <v>162</v>
       </c>
-      <c r="L20" s="51"/>
+      <c r="L20" s="52"/>
       <c r="M20" s="5" t="s">
         <v>128</v>
       </c>
@@ -2112,13 +2133,13 @@
       <c r="C21" s="15"/>
       <c r="D21" s="15"/>
       <c r="E21" s="15"/>
-      <c r="G21" s="53"/>
+      <c r="G21" s="54"/>
       <c r="H21" s="3" t="s">
         <v>26</v>
       </c>
       <c r="I21" s="3"/>
       <c r="J21" s="4"/>
-      <c r="L21" s="52" t="s">
+      <c r="L21" s="51" t="s">
         <v>79</v>
       </c>
       <c r="M21" s="7" t="s">
@@ -2136,7 +2157,7 @@
         <v>114</v>
       </c>
       <c r="E22" s="42"/>
-      <c r="G22" s="54" t="s">
+      <c r="G22" s="50" t="s">
         <v>56</v>
       </c>
       <c r="H22" s="3" t="s">
@@ -2144,7 +2165,7 @@
       </c>
       <c r="I22" s="3"/>
       <c r="J22" s="4"/>
-      <c r="L22" s="52"/>
+      <c r="L22" s="51"/>
       <c r="M22" s="3" t="s">
         <v>25</v>
       </c>
@@ -2158,7 +2179,7 @@
       <c r="C23" s="15"/>
       <c r="D23" s="15"/>
       <c r="E23" s="15"/>
-      <c r="G23" s="52"/>
+      <c r="G23" s="51"/>
       <c r="H23" s="3" t="s">
         <v>25</v>
       </c>
@@ -2168,7 +2189,7 @@
       <c r="J23" s="4" t="s">
         <v>165</v>
       </c>
-      <c r="L23" s="51"/>
+      <c r="L23" s="52"/>
       <c r="M23" s="5" t="s">
         <v>26</v>
       </c>
@@ -2176,7 +2197,7 @@
       <c r="O23" s="6"/>
     </row>
     <row r="24" spans="2:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B24" s="50" t="s">
+      <c r="B24" s="53" t="s">
         <v>28</v>
       </c>
       <c r="C24" s="12" t="s">
@@ -2184,7 +2205,7 @@
       </c>
       <c r="D24" s="12"/>
       <c r="E24" s="13"/>
-      <c r="G24" s="53"/>
+      <c r="G24" s="54"/>
       <c r="H24" s="3" t="s">
         <v>26</v>
       </c>
@@ -2192,7 +2213,7 @@
       <c r="J24" s="4"/>
     </row>
     <row r="25" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B25" s="52"/>
+      <c r="B25" s="51"/>
       <c r="C25" s="3" t="s">
         <v>25</v>
       </c>
@@ -2200,7 +2221,7 @@
         <v>5</v>
       </c>
       <c r="E25" s="4"/>
-      <c r="G25" s="54" t="s">
+      <c r="G25" s="50" t="s">
         <v>57</v>
       </c>
       <c r="H25" s="3" t="s">
@@ -2208,7 +2229,7 @@
       </c>
       <c r="I25" s="3"/>
       <c r="J25" s="4"/>
-      <c r="L25" s="50" t="s">
+      <c r="L25" s="53" t="s">
         <v>80</v>
       </c>
       <c r="M25" s="38" t="s">
@@ -2220,13 +2241,13 @@
       <c r="O25" s="39"/>
     </row>
     <row r="26" spans="2:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B26" s="51"/>
+      <c r="B26" s="52"/>
       <c r="C26" s="5" t="s">
         <v>26</v>
       </c>
       <c r="D26" s="5"/>
       <c r="E26" s="6"/>
-      <c r="G26" s="52"/>
+      <c r="G26" s="51"/>
       <c r="H26" s="3" t="s">
         <v>25</v>
       </c>
@@ -2234,7 +2255,7 @@
         <v>100</v>
       </c>
       <c r="J26" s="4"/>
-      <c r="L26" s="51"/>
+      <c r="L26" s="52"/>
       <c r="M26" s="5" t="s">
         <v>128</v>
       </c>
@@ -2248,7 +2269,7 @@
       <c r="C27" s="15"/>
       <c r="D27" s="15"/>
       <c r="E27" s="15"/>
-      <c r="G27" s="53"/>
+      <c r="G27" s="54"/>
       <c r="H27" s="3" t="s">
         <v>26</v>
       </c>
@@ -2256,7 +2277,7 @@
       <c r="J27" s="4"/>
     </row>
     <row r="28" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B28" s="50" t="s">
+      <c r="B28" s="53" t="s">
         <v>29</v>
       </c>
       <c r="C28" s="12" t="s">
@@ -2266,7 +2287,7 @@
         <v>6</v>
       </c>
       <c r="E28" s="13"/>
-      <c r="G28" s="54" t="s">
+      <c r="G28" s="50" t="s">
         <v>58</v>
       </c>
       <c r="H28" s="3" t="s">
@@ -2274,7 +2295,7 @@
       </c>
       <c r="I28" s="3"/>
       <c r="J28" s="4"/>
-      <c r="L28" s="50" t="s">
+      <c r="L28" s="53" t="s">
         <v>81</v>
       </c>
       <c r="M28" s="38" t="s">
@@ -2286,7 +2307,7 @@
       <c r="O28" s="39"/>
     </row>
     <row r="29" spans="2:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B29" s="52"/>
+      <c r="B29" s="51"/>
       <c r="C29" s="3" t="s">
         <v>25</v>
       </c>
@@ -2294,7 +2315,7 @@
         <v>9</v>
       </c>
       <c r="E29" s="4"/>
-      <c r="G29" s="52"/>
+      <c r="G29" s="51"/>
       <c r="H29" s="3" t="s">
         <v>25</v>
       </c>
@@ -2302,7 +2323,7 @@
         <v>101</v>
       </c>
       <c r="J29" s="4"/>
-      <c r="L29" s="51"/>
+      <c r="L29" s="52"/>
       <c r="M29" s="5" t="s">
         <v>128</v>
       </c>
@@ -2312,7 +2333,7 @@
       <c r="O29" s="6"/>
     </row>
     <row r="30" spans="2:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B30" s="53"/>
+      <c r="B30" s="54"/>
       <c r="C30" s="3" t="s">
         <v>26</v>
       </c>
@@ -2320,7 +2341,7 @@
         <v>8</v>
       </c>
       <c r="E30" s="4"/>
-      <c r="G30" s="51"/>
+      <c r="G30" s="52"/>
       <c r="H30" s="5" t="s">
         <v>26</v>
       </c>
@@ -2328,7 +2349,7 @@
       <c r="J30" s="6"/>
     </row>
     <row r="31" spans="2:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B31" s="54" t="s">
+      <c r="B31" s="50" t="s">
         <v>30</v>
       </c>
       <c r="C31" s="3" t="s">
@@ -2336,7 +2357,7 @@
       </c>
       <c r="D31" s="3"/>
       <c r="E31" s="4"/>
-      <c r="L31" s="50" t="s">
+      <c r="L31" s="53" t="s">
         <v>82</v>
       </c>
       <c r="M31" s="12" t="s">
@@ -2348,7 +2369,7 @@
       <c r="O31" s="13"/>
     </row>
     <row r="32" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B32" s="52"/>
+      <c r="B32" s="51"/>
       <c r="C32" s="3" t="s">
         <v>25</v>
       </c>
@@ -2361,10 +2382,10 @@
       </c>
       <c r="H32" s="38"/>
       <c r="I32" s="38" t="s">
-        <v>207</v>
+        <v>204</v>
       </c>
       <c r="J32" s="39"/>
-      <c r="L32" s="52"/>
+      <c r="L32" s="51"/>
       <c r="M32" s="3" t="s">
         <v>25</v>
       </c>
@@ -2376,7 +2397,7 @@
       </c>
     </row>
     <row r="33" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B33" s="53"/>
+      <c r="B33" s="54"/>
       <c r="C33" s="3" t="s">
         <v>26</v>
       </c>
@@ -2387,20 +2408,20 @@
       </c>
       <c r="H33" s="3"/>
       <c r="I33" s="3" t="s">
-        <v>208</v>
+        <v>205</v>
       </c>
       <c r="J33" s="4"/>
-      <c r="L33" s="53"/>
+      <c r="L33" s="54"/>
       <c r="M33" s="3" t="s">
         <v>26</v>
       </c>
       <c r="N33" s="3" t="s">
-        <v>220</v>
+        <v>217</v>
       </c>
       <c r="O33" s="4"/>
     </row>
     <row r="34" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B34" s="54" t="s">
+      <c r="B34" s="50" t="s">
         <v>31</v>
       </c>
       <c r="C34" s="3" t="s">
@@ -2413,10 +2434,10 @@
       </c>
       <c r="H34" s="3"/>
       <c r="I34" s="3" t="s">
-        <v>209</v>
+        <v>206</v>
       </c>
       <c r="J34" s="4"/>
-      <c r="L34" s="54" t="s">
+      <c r="L34" s="50" t="s">
         <v>182</v>
       </c>
       <c r="M34" s="3" t="s">
@@ -2426,7 +2447,7 @@
       <c r="O34" s="4"/>
     </row>
     <row r="35" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B35" s="52"/>
+      <c r="B35" s="51"/>
       <c r="C35" s="3" t="s">
         <v>25</v>
       </c>
@@ -2441,10 +2462,10 @@
       </c>
       <c r="H35" s="3"/>
       <c r="I35" s="3" t="s">
-        <v>210</v>
+        <v>207</v>
       </c>
       <c r="J35" s="4"/>
-      <c r="L35" s="52"/>
+      <c r="L35" s="51"/>
       <c r="M35" s="3" t="s">
         <v>25</v>
       </c>
@@ -2456,7 +2477,7 @@
       </c>
     </row>
     <row r="36" spans="2:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B36" s="53"/>
+      <c r="B36" s="54"/>
       <c r="C36" s="3" t="s">
         <v>26</v>
       </c>
@@ -2468,7 +2489,7 @@
       <c r="H36" s="5"/>
       <c r="I36" s="5"/>
       <c r="J36" s="6"/>
-      <c r="L36" s="53"/>
+      <c r="L36" s="54"/>
       <c r="M36" s="3" t="s">
         <v>26</v>
       </c>
@@ -2476,7 +2497,7 @@
       <c r="O36" s="4"/>
     </row>
     <row r="37" spans="2:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B37" s="54" t="s">
+      <c r="B37" s="50" t="s">
         <v>32</v>
       </c>
       <c r="C37" s="3" t="s">
@@ -2488,7 +2509,7 @@
       <c r="E37" s="4" t="s">
         <v>143</v>
       </c>
-      <c r="L37" s="54" t="s">
+      <c r="L37" s="50" t="s">
         <v>83</v>
       </c>
       <c r="M37" s="3" t="s">
@@ -2498,7 +2519,7 @@
       <c r="O37" s="4"/>
     </row>
     <row r="38" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B38" s="52"/>
+      <c r="B38" s="51"/>
       <c r="C38" s="3" t="s">
         <v>25</v>
       </c>
@@ -2508,7 +2529,7 @@
       <c r="E38" s="4" t="s">
         <v>141</v>
       </c>
-      <c r="G38" s="50" t="s">
+      <c r="G38" s="53" t="s">
         <v>64</v>
       </c>
       <c r="H38" s="12" t="s">
@@ -2520,7 +2541,7 @@
       <c r="J38" s="13" t="s">
         <v>166</v>
       </c>
-      <c r="L38" s="52"/>
+      <c r="L38" s="51"/>
       <c r="M38" s="3" t="s">
         <v>25</v>
       </c>
@@ -2528,13 +2549,13 @@
       <c r="O38" s="4"/>
     </row>
     <row r="39" spans="2:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B39" s="51"/>
+      <c r="B39" s="52"/>
       <c r="C39" s="5" t="s">
         <v>26</v>
       </c>
       <c r="D39" s="5"/>
       <c r="E39" s="6"/>
-      <c r="G39" s="52"/>
+      <c r="G39" s="51"/>
       <c r="H39" s="3" t="s">
         <v>25</v>
       </c>
@@ -2544,7 +2565,7 @@
       <c r="J39" s="4" t="s">
         <v>167</v>
       </c>
-      <c r="L39" s="53"/>
+      <c r="L39" s="54"/>
       <c r="M39" s="3" t="s">
         <v>26</v>
       </c>
@@ -2556,7 +2577,7 @@
       <c r="C40" s="15"/>
       <c r="D40" s="15"/>
       <c r="E40" s="15"/>
-      <c r="G40" s="53"/>
+      <c r="G40" s="54"/>
       <c r="H40" s="3" t="s">
         <v>26</v>
       </c>
@@ -2566,7 +2587,7 @@
       <c r="J40" s="4" t="s">
         <v>168</v>
       </c>
-      <c r="L40" s="54" t="s">
+      <c r="L40" s="50" t="s">
         <v>84</v>
       </c>
       <c r="M40" s="3" t="s">
@@ -2578,7 +2599,7 @@
       <c r="O40" s="4"/>
     </row>
     <row r="41" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B41" s="50" t="s">
+      <c r="B41" s="53" t="s">
         <v>33</v>
       </c>
       <c r="C41" s="12" t="s">
@@ -2598,7 +2619,7 @@
       <c r="J41" s="4" t="s">
         <v>169</v>
       </c>
-      <c r="L41" s="52"/>
+      <c r="L41" s="51"/>
       <c r="M41" s="3" t="s">
         <v>25</v>
       </c>
@@ -2610,7 +2631,7 @@
       </c>
     </row>
     <row r="42" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B42" s="52"/>
+      <c r="B42" s="51"/>
       <c r="C42" s="3" t="s">
         <v>25</v>
       </c>
@@ -2618,7 +2639,7 @@
         <v>11</v>
       </c>
       <c r="E42" s="4"/>
-      <c r="G42" s="52" t="s">
+      <c r="G42" s="51" t="s">
         <v>66</v>
       </c>
       <c r="H42" s="7" t="s">
@@ -2626,7 +2647,7 @@
       </c>
       <c r="I42" s="7"/>
       <c r="J42" s="8"/>
-      <c r="L42" s="53"/>
+      <c r="L42" s="54"/>
       <c r="M42" s="3" t="s">
         <v>26</v>
       </c>
@@ -2636,7 +2657,7 @@
       <c r="O42" s="4"/>
     </row>
     <row r="43" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B43" s="53"/>
+      <c r="B43" s="54"/>
       <c r="C43" s="3" t="s">
         <v>26</v>
       </c>
@@ -2644,7 +2665,7 @@
         <v>11</v>
       </c>
       <c r="E43" s="4"/>
-      <c r="G43" s="52"/>
+      <c r="G43" s="51"/>
       <c r="H43" s="3" t="s">
         <v>25</v>
       </c>
@@ -2652,7 +2673,7 @@
         <v>67</v>
       </c>
       <c r="J43" s="4"/>
-      <c r="L43" s="52" t="s">
+      <c r="L43" s="51" t="s">
         <v>184</v>
       </c>
       <c r="M43" s="3" t="s">
@@ -2662,7 +2683,7 @@
       <c r="O43" s="4"/>
     </row>
     <row r="44" spans="2:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B44" s="54" t="s">
+      <c r="B44" s="50" t="s">
         <v>34</v>
       </c>
       <c r="C44" s="3" t="s">
@@ -2670,13 +2691,13 @@
       </c>
       <c r="D44" s="3"/>
       <c r="E44" s="4"/>
-      <c r="G44" s="51"/>
+      <c r="G44" s="52"/>
       <c r="H44" s="5" t="s">
         <v>26</v>
       </c>
       <c r="I44" s="5"/>
       <c r="J44" s="6"/>
-      <c r="L44" s="52"/>
+      <c r="L44" s="51"/>
       <c r="M44" s="3" t="s">
         <v>25</v>
       </c>
@@ -2688,7 +2709,7 @@
       </c>
     </row>
     <row r="45" spans="2:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B45" s="52"/>
+      <c r="B45" s="51"/>
       <c r="C45" s="3" t="s">
         <v>25</v>
       </c>
@@ -2696,7 +2717,7 @@
         <v>12</v>
       </c>
       <c r="E45" s="4"/>
-      <c r="L45" s="51"/>
+      <c r="L45" s="52"/>
       <c r="M45" s="5" t="s">
         <v>26</v>
       </c>
@@ -2706,7 +2727,7 @@
       <c r="O45" s="6"/>
     </row>
     <row r="46" spans="2:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B46" s="53"/>
+      <c r="B46" s="54"/>
       <c r="C46" s="3" t="s">
         <v>26</v>
       </c>
@@ -2714,7 +2735,7 @@
         <v>13</v>
       </c>
       <c r="E46" s="4"/>
-      <c r="G46" s="50" t="s">
+      <c r="G46" s="53" t="s">
         <v>68</v>
       </c>
       <c r="H46" s="31" t="s">
@@ -2726,7 +2747,7 @@
       <c r="J46" s="32"/>
     </row>
     <row r="47" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B47" s="54" t="s">
+      <c r="B47" s="50" t="s">
         <v>35</v>
       </c>
       <c r="C47" s="3" t="s">
@@ -2734,13 +2755,13 @@
       </c>
       <c r="D47" s="3"/>
       <c r="E47" s="4"/>
-      <c r="G47" s="52"/>
+      <c r="G47" s="51"/>
       <c r="H47" s="3" t="s">
         <v>25</v>
       </c>
       <c r="I47" s="15"/>
       <c r="J47" s="4"/>
-      <c r="L47" s="50" t="s">
+      <c r="L47" s="53" t="s">
         <v>85</v>
       </c>
       <c r="M47" s="12" t="s">
@@ -2750,7 +2771,7 @@
       <c r="O47" s="13"/>
     </row>
     <row r="48" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B48" s="52"/>
+      <c r="B48" s="51"/>
       <c r="C48" s="3" t="s">
         <v>25</v>
       </c>
@@ -2758,7 +2779,7 @@
         <v>14</v>
       </c>
       <c r="E48" s="4"/>
-      <c r="G48" s="53"/>
+      <c r="G48" s="54"/>
       <c r="H48" s="3" t="s">
         <v>26</v>
       </c>
@@ -2768,7 +2789,7 @@
       <c r="J48" s="4" t="s">
         <v>171</v>
       </c>
-      <c r="L48" s="52"/>
+      <c r="L48" s="51"/>
       <c r="M48" s="3" t="s">
         <v>25</v>
       </c>
@@ -2778,7 +2799,7 @@
       <c r="O48" s="4"/>
     </row>
     <row r="49" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B49" s="53"/>
+      <c r="B49" s="54"/>
       <c r="C49" s="3" t="s">
         <v>26</v>
       </c>
@@ -2786,7 +2807,7 @@
         <v>15</v>
       </c>
       <c r="E49" s="4"/>
-      <c r="G49" s="54" t="s">
+      <c r="G49" s="50" t="s">
         <v>69</v>
       </c>
       <c r="H49" s="3" t="s">
@@ -2794,7 +2815,7 @@
       </c>
       <c r="I49" s="3"/>
       <c r="J49" s="4"/>
-      <c r="L49" s="53"/>
+      <c r="L49" s="54"/>
       <c r="M49" s="3" t="s">
         <v>26</v>
       </c>
@@ -2802,7 +2823,7 @@
       <c r="O49" s="4"/>
     </row>
     <row r="50" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B50" s="54" t="s">
+      <c r="B50" s="50" t="s">
         <v>36</v>
       </c>
       <c r="C50" s="3" t="s">
@@ -2810,13 +2831,13 @@
       </c>
       <c r="D50" s="3"/>
       <c r="E50" s="4"/>
-      <c r="G50" s="52"/>
+      <c r="G50" s="51"/>
       <c r="H50" s="3" t="s">
         <v>25</v>
       </c>
       <c r="I50" s="3"/>
       <c r="J50" s="4"/>
-      <c r="L50" s="54" t="s">
+      <c r="L50" s="50" t="s">
         <v>86</v>
       </c>
       <c r="M50" s="3" t="s">
@@ -2826,7 +2847,7 @@
       <c r="O50" s="4"/>
     </row>
     <row r="51" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B51" s="52"/>
+      <c r="B51" s="51"/>
       <c r="C51" s="3" t="s">
         <v>25</v>
       </c>
@@ -2834,13 +2855,13 @@
         <v>16</v>
       </c>
       <c r="E51" s="4"/>
-      <c r="G51" s="53"/>
+      <c r="G51" s="54"/>
       <c r="H51" s="3" t="s">
         <v>26</v>
       </c>
       <c r="I51" s="3"/>
       <c r="J51" s="4"/>
-      <c r="L51" s="52"/>
+      <c r="L51" s="51"/>
       <c r="M51" s="3" t="s">
         <v>25</v>
       </c>
@@ -2850,7 +2871,7 @@
       <c r="O51" s="4"/>
     </row>
     <row r="52" spans="2:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B52" s="51"/>
+      <c r="B52" s="52"/>
       <c r="C52" s="5" t="s">
         <v>26</v>
       </c>
@@ -2858,7 +2879,7 @@
         <v>17</v>
       </c>
       <c r="E52" s="6"/>
-      <c r="G52" s="54" t="s">
+      <c r="G52" s="50" t="s">
         <v>70</v>
       </c>
       <c r="H52" s="3" t="s">
@@ -2868,7 +2889,7 @@
         <v>103</v>
       </c>
       <c r="J52" s="4"/>
-      <c r="L52" s="51"/>
+      <c r="L52" s="52"/>
       <c r="M52" s="5" t="s">
         <v>26</v>
       </c>
@@ -2880,14 +2901,14 @@
       <c r="C53" s="15"/>
       <c r="D53" s="15"/>
       <c r="E53" s="15"/>
-      <c r="G53" s="52"/>
+      <c r="G53" s="51"/>
       <c r="H53" s="3" t="s">
         <v>25</v>
       </c>
       <c r="J53" s="4"/>
     </row>
     <row r="54" spans="2:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B54" s="50" t="s">
+      <c r="B54" s="53" t="s">
         <v>37</v>
       </c>
       <c r="C54" s="12" t="s">
@@ -2895,13 +2916,13 @@
       </c>
       <c r="D54" s="12"/>
       <c r="E54" s="13"/>
-      <c r="G54" s="51"/>
+      <c r="G54" s="52"/>
       <c r="H54" s="5" t="s">
         <v>26</v>
       </c>
       <c r="I54" s="5"/>
       <c r="J54" s="6"/>
-      <c r="L54" s="50" t="s">
+      <c r="L54" s="53" t="s">
         <v>87</v>
       </c>
       <c r="M54" s="12" t="s">
@@ -2911,7 +2932,7 @@
       <c r="O54" s="13"/>
     </row>
     <row r="55" spans="2:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B55" s="52"/>
+      <c r="B55" s="51"/>
       <c r="C55" s="3" t="s">
         <v>25</v>
       </c>
@@ -2919,7 +2940,7 @@
         <v>146</v>
       </c>
       <c r="E55" s="4"/>
-      <c r="L55" s="52"/>
+      <c r="L55" s="51"/>
       <c r="M55" s="3" t="s">
         <v>25</v>
       </c>
@@ -2931,13 +2952,13 @@
       </c>
     </row>
     <row r="56" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B56" s="53"/>
+      <c r="B56" s="54"/>
       <c r="C56" s="3" t="s">
         <v>26</v>
       </c>
       <c r="D56" s="3"/>
       <c r="E56" s="4"/>
-      <c r="G56" s="50" t="s">
+      <c r="G56" s="53" t="s">
         <v>71</v>
       </c>
       <c r="H56" s="12" t="s">
@@ -2945,7 +2966,7 @@
       </c>
       <c r="I56" s="12"/>
       <c r="J56" s="13"/>
-      <c r="L56" s="53"/>
+      <c r="L56" s="54"/>
       <c r="M56" s="3" t="s">
         <v>26</v>
       </c>
@@ -2953,7 +2974,7 @@
       <c r="O56" s="4"/>
     </row>
     <row r="57" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B57" s="54" t="s">
+      <c r="B57" s="50" t="s">
         <v>38</v>
       </c>
       <c r="C57" s="3" t="s">
@@ -2961,7 +2982,7 @@
       </c>
       <c r="D57" s="3"/>
       <c r="E57" s="4"/>
-      <c r="G57" s="52"/>
+      <c r="G57" s="51"/>
       <c r="H57" s="3" t="s">
         <v>25</v>
       </c>
@@ -2969,7 +2990,7 @@
         <v>172</v>
       </c>
       <c r="J57" s="4"/>
-      <c r="L57" s="54" t="s">
+      <c r="L57" s="50" t="s">
         <v>88</v>
       </c>
       <c r="M57" s="3" t="s">
@@ -2979,7 +3000,7 @@
       <c r="O57" s="4"/>
     </row>
     <row r="58" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B58" s="52"/>
+      <c r="B58" s="51"/>
       <c r="C58" s="3" t="s">
         <v>25</v>
       </c>
@@ -2987,13 +3008,13 @@
         <v>147</v>
       </c>
       <c r="E58" s="4"/>
-      <c r="G58" s="53"/>
+      <c r="G58" s="54"/>
       <c r="H58" s="3" t="s">
         <v>26</v>
       </c>
       <c r="I58" s="3"/>
       <c r="J58" s="4"/>
-      <c r="L58" s="52"/>
+      <c r="L58" s="51"/>
       <c r="M58" s="3" t="s">
         <v>25</v>
       </c>
@@ -3001,13 +3022,13 @@
       <c r="O58" s="4"/>
     </row>
     <row r="59" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B59" s="53"/>
+      <c r="B59" s="54"/>
       <c r="C59" s="3" t="s">
         <v>26</v>
       </c>
       <c r="D59" s="3"/>
       <c r="E59" s="4"/>
-      <c r="G59" s="54" t="s">
+      <c r="G59" s="50" t="s">
         <v>72</v>
       </c>
       <c r="H59" s="3" t="s">
@@ -3015,7 +3036,7 @@
       </c>
       <c r="I59" s="3"/>
       <c r="J59" s="4"/>
-      <c r="L59" s="53"/>
+      <c r="L59" s="54"/>
       <c r="M59" s="3" t="s">
         <v>26</v>
       </c>
@@ -3023,7 +3044,7 @@
       <c r="O59" s="4"/>
     </row>
     <row r="60" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B60" s="54" t="s">
+      <c r="B60" s="50" t="s">
         <v>39</v>
       </c>
       <c r="C60" s="3" t="s">
@@ -3031,7 +3052,7 @@
       </c>
       <c r="D60" s="3"/>
       <c r="E60" s="4"/>
-      <c r="G60" s="52"/>
+      <c r="G60" s="51"/>
       <c r="H60" s="3" t="s">
         <v>25</v>
       </c>
@@ -3039,7 +3060,7 @@
         <v>173</v>
       </c>
       <c r="J60" s="4"/>
-      <c r="L60" s="54" t="s">
+      <c r="L60" s="50" t="s">
         <v>89</v>
       </c>
       <c r="M60" s="3" t="s">
@@ -3049,7 +3070,7 @@
       <c r="O60" s="4"/>
     </row>
     <row r="61" spans="2:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B61" s="52"/>
+      <c r="B61" s="51"/>
       <c r="C61" s="3" t="s">
         <v>25</v>
       </c>
@@ -3057,13 +3078,13 @@
         <v>148</v>
       </c>
       <c r="E61" s="4"/>
-      <c r="G61" s="51"/>
+      <c r="G61" s="52"/>
       <c r="H61" s="5" t="s">
         <v>26</v>
       </c>
       <c r="I61" s="5"/>
       <c r="J61" s="6"/>
-      <c r="L61" s="52"/>
+      <c r="L61" s="51"/>
       <c r="M61" s="3" t="s">
         <v>25</v>
       </c>
@@ -3075,13 +3096,13 @@
       </c>
     </row>
     <row r="62" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B62" s="53"/>
+      <c r="B62" s="54"/>
       <c r="C62" s="3" t="s">
         <v>26</v>
       </c>
       <c r="D62" s="3"/>
       <c r="E62" s="4"/>
-      <c r="L62" s="53"/>
+      <c r="L62" s="54"/>
       <c r="M62" s="3" t="s">
         <v>26</v>
       </c>
@@ -3089,7 +3110,7 @@
       <c r="O62" s="4"/>
     </row>
     <row r="63" spans="2:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B63" s="54" t="s">
+      <c r="B63" s="50" t="s">
         <v>40</v>
       </c>
       <c r="C63" s="3" t="s">
@@ -3109,7 +3130,7 @@
       </c>
     </row>
     <row r="64" spans="2:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B64" s="52"/>
+      <c r="B64" s="51"/>
       <c r="C64" s="3" t="s">
         <v>25</v>
       </c>
@@ -3119,13 +3140,13 @@
       <c r="E64" s="4"/>
     </row>
     <row r="65" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B65" s="51"/>
+      <c r="B65" s="52"/>
       <c r="C65" s="5" t="s">
         <v>26</v>
       </c>
       <c r="D65" s="5"/>
       <c r="E65" s="6"/>
-      <c r="L65" s="50" t="s">
+      <c r="L65" s="53" t="s">
         <v>91</v>
       </c>
       <c r="M65" s="12" t="s">
@@ -3143,7 +3164,7 @@
       <c r="C66" s="15"/>
       <c r="D66" s="15"/>
       <c r="E66" s="15"/>
-      <c r="L66" s="52"/>
+      <c r="L66" s="51"/>
       <c r="M66" s="3" t="s">
         <v>25</v>
       </c>
@@ -3155,7 +3176,7 @@
       </c>
     </row>
     <row r="67" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="B67" s="50" t="s">
+      <c r="B67" s="53" t="s">
         <v>41</v>
       </c>
       <c r="C67" s="12" t="s">
@@ -3167,7 +3188,7 @@
       <c r="E67" s="13" t="s">
         <v>151</v>
       </c>
-      <c r="L67" s="53"/>
+      <c r="L67" s="54"/>
       <c r="M67" s="3" t="s">
         <v>26</v>
       </c>
@@ -3179,7 +3200,7 @@
       </c>
     </row>
     <row r="68" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="B68" s="52"/>
+      <c r="B68" s="51"/>
       <c r="C68" s="3" t="s">
         <v>25</v>
       </c>
@@ -3189,7 +3210,7 @@
       <c r="E68" s="4" t="s">
         <v>153</v>
       </c>
-      <c r="L68" s="54" t="s">
+      <c r="L68" s="50" t="s">
         <v>92</v>
       </c>
       <c r="M68" s="3" t="s">
@@ -3199,7 +3220,7 @@
       <c r="O68" s="4"/>
     </row>
     <row r="69" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="B69" s="53"/>
+      <c r="B69" s="54"/>
       <c r="C69" s="3" t="s">
         <v>26</v>
       </c>
@@ -3207,7 +3228,7 @@
         <v>18</v>
       </c>
       <c r="E69" s="27"/>
-      <c r="L69" s="52"/>
+      <c r="L69" s="51"/>
       <c r="M69" s="3" t="s">
         <v>25</v>
       </c>
@@ -3215,7 +3236,7 @@
       <c r="O69" s="4"/>
     </row>
     <row r="70" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="B70" s="54" t="s">
+      <c r="B70" s="50" t="s">
         <v>42</v>
       </c>
       <c r="C70" s="3" t="s">
@@ -3223,7 +3244,7 @@
       </c>
       <c r="D70" s="3"/>
       <c r="E70" s="4"/>
-      <c r="L70" s="53"/>
+      <c r="L70" s="54"/>
       <c r="M70" s="3" t="s">
         <v>26</v>
       </c>
@@ -3231,7 +3252,7 @@
       <c r="O70" s="4"/>
     </row>
     <row r="71" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="B71" s="52"/>
+      <c r="B71" s="51"/>
       <c r="C71" s="3" t="s">
         <v>25</v>
       </c>
@@ -3239,7 +3260,7 @@
         <v>154</v>
       </c>
       <c r="E71" s="4"/>
-      <c r="L71" s="54" t="s">
+      <c r="L71" s="50" t="s">
         <v>93</v>
       </c>
       <c r="M71" s="3" t="s">
@@ -3249,7 +3270,7 @@
       <c r="O71" s="4"/>
     </row>
     <row r="72" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="B72" s="53"/>
+      <c r="B72" s="54"/>
       <c r="C72" s="3" t="s">
         <v>26</v>
       </c>
@@ -3257,17 +3278,17 @@
         <v>19</v>
       </c>
       <c r="E72" s="27"/>
-      <c r="L72" s="52"/>
+      <c r="L72" s="51"/>
       <c r="M72" s="3" t="s">
         <v>25</v>
       </c>
       <c r="N72" s="3" t="s">
-        <v>219</v>
+        <v>216</v>
       </c>
       <c r="O72" s="4"/>
     </row>
     <row r="73" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B73" s="54" t="s">
+      <c r="B73" s="50" t="s">
         <v>43</v>
       </c>
       <c r="C73" s="3" t="s">
@@ -3275,7 +3296,7 @@
       </c>
       <c r="D73" s="3"/>
       <c r="E73" s="4"/>
-      <c r="L73" s="51"/>
+      <c r="L73" s="52"/>
       <c r="M73" s="5" t="s">
         <v>26</v>
       </c>
@@ -3283,7 +3304,7 @@
       <c r="O73" s="6"/>
     </row>
     <row r="74" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B74" s="52"/>
+      <c r="B74" s="51"/>
       <c r="C74" s="3" t="s">
         <v>25</v>
       </c>
@@ -3295,7 +3316,7 @@
       </c>
     </row>
     <row r="75" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="B75" s="53"/>
+      <c r="B75" s="54"/>
       <c r="C75" s="3" t="s">
         <v>26</v>
       </c>
@@ -3303,17 +3324,19 @@
         <v>20</v>
       </c>
       <c r="E75" s="27"/>
-      <c r="L75" s="50" t="s">
+      <c r="L75" s="53" t="s">
         <v>94</v>
       </c>
       <c r="M75" s="12" t="s">
         <v>24</v>
       </c>
-      <c r="N75" s="12"/>
+      <c r="N75" s="12" t="s">
+        <v>220</v>
+      </c>
       <c r="O75" s="13"/>
     </row>
     <row r="76" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="B76" s="54" t="s">
+      <c r="B76" s="50" t="s">
         <v>118</v>
       </c>
       <c r="C76" s="3" t="s">
@@ -3323,17 +3346,19 @@
         <v>0</v>
       </c>
       <c r="E76" s="4"/>
-      <c r="L76" s="52"/>
+      <c r="L76" s="51"/>
       <c r="M76" s="3" t="s">
         <v>25</v>
       </c>
       <c r="N76" s="3" t="s">
+        <v>106</v>
+      </c>
+      <c r="O76" s="4" t="s">
         <v>199</v>
       </c>
-      <c r="O76" s="4"/>
     </row>
     <row r="77" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="B77" s="52"/>
+      <c r="B77" s="51"/>
       <c r="C77" s="3" t="s">
         <v>25</v>
       </c>
@@ -3343,20 +3368,18 @@
       <c r="E77" s="4" t="s">
         <v>156</v>
       </c>
-      <c r="L77" s="53"/>
+      <c r="L77" s="54"/>
       <c r="M77" s="3" t="s">
         <v>26</v>
       </c>
       <c r="N77" s="3" t="s">
-        <v>106</v>
-      </c>
-      <c r="O77" s="4" t="s">
-        <v>200</v>
-      </c>
+        <v>219</v>
+      </c>
+      <c r="O77" s="4"/>
     </row>
     <row r="78" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A78" s="2"/>
-      <c r="B78" s="53"/>
+      <c r="B78" s="54"/>
       <c r="C78" s="3" t="s">
         <v>26</v>
       </c>
@@ -3365,7 +3388,7 @@
       </c>
       <c r="E78" s="4"/>
       <c r="F78" s="2"/>
-      <c r="L78" s="54" t="s">
+      <c r="L78" s="50" t="s">
         <v>95</v>
       </c>
       <c r="M78" s="3" t="s">
@@ -3376,7 +3399,7 @@
     </row>
     <row r="79" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A79" s="2"/>
-      <c r="B79" s="54" t="s">
+      <c r="B79" s="50" t="s">
         <v>44</v>
       </c>
       <c r="C79" s="3" t="s">
@@ -3385,7 +3408,7 @@
       <c r="D79" s="3"/>
       <c r="E79" s="4"/>
       <c r="F79" s="2"/>
-      <c r="L79" s="52"/>
+      <c r="L79" s="51"/>
       <c r="M79" s="3" t="s">
         <v>25</v>
       </c>
@@ -3394,7 +3417,7 @@
     </row>
     <row r="80" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A80" s="2"/>
-      <c r="B80" s="52"/>
+      <c r="B80" s="51"/>
       <c r="C80" s="3" t="s">
         <v>25</v>
       </c>
@@ -3403,7 +3426,7 @@
       </c>
       <c r="E80" s="4"/>
       <c r="F80" s="2"/>
-      <c r="L80" s="51"/>
+      <c r="L80" s="52"/>
       <c r="M80" s="5" t="s">
         <v>26</v>
       </c>
@@ -3411,7 +3434,7 @@
       <c r="O80" s="6"/>
     </row>
     <row r="81" spans="2:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B81" s="53"/>
+      <c r="B81" s="54"/>
       <c r="C81" s="3" t="s">
         <v>26</v>
       </c>
@@ -3421,7 +3444,7 @@
       <c r="E81" s="27"/>
     </row>
     <row r="82" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B82" s="54" t="s">
+      <c r="B82" s="50" t="s">
         <v>22</v>
       </c>
       <c r="C82" s="3" t="s">
@@ -3433,19 +3456,21 @@
       <c r="E82" s="4" t="s">
         <v>158</v>
       </c>
-      <c r="L82" s="50" t="s">
+      <c r="L82" s="53" t="s">
         <v>96</v>
       </c>
       <c r="M82" s="12" t="s">
         <v>24</v>
       </c>
       <c r="N82" s="12" t="s">
-        <v>201</v>
-      </c>
-      <c r="O82" s="13"/>
+        <v>221</v>
+      </c>
+      <c r="O82" s="13" t="s">
+        <v>224</v>
+      </c>
     </row>
     <row r="83" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B83" s="52"/>
+      <c r="B83" s="51"/>
       <c r="C83" s="3" t="s">
         <v>25</v>
       </c>
@@ -3455,17 +3480,19 @@
       <c r="E83" s="4" t="s">
         <v>159</v>
       </c>
-      <c r="L83" s="52"/>
+      <c r="L83" s="51"/>
       <c r="M83" s="3" t="s">
         <v>25</v>
       </c>
       <c r="N83" s="3" t="s">
-        <v>202</v>
-      </c>
-      <c r="O83" s="4"/>
+        <v>222</v>
+      </c>
+      <c r="O83" s="4" t="s">
+        <v>225</v>
+      </c>
     </row>
     <row r="84" spans="2:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B84" s="51"/>
+      <c r="B84" s="52"/>
       <c r="C84" s="5" t="s">
         <v>26</v>
       </c>
@@ -3475,15 +3502,19 @@
       <c r="E84" s="6" t="s">
         <v>160</v>
       </c>
-      <c r="L84" s="53"/>
+      <c r="L84" s="54"/>
       <c r="M84" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="N84" s="3"/>
-      <c r="O84" s="4"/>
+      <c r="N84" s="3" t="s">
+        <v>223</v>
+      </c>
+      <c r="O84" s="4" t="s">
+        <v>226</v>
+      </c>
     </row>
     <row r="85" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="L85" s="54" t="s">
+      <c r="L85" s="50" t="s">
         <v>107</v>
       </c>
       <c r="M85" s="3" t="s">
@@ -3493,7 +3524,7 @@
       <c r="O85" s="4"/>
     </row>
     <row r="86" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="L86" s="52"/>
+      <c r="L86" s="51"/>
       <c r="M86" s="3" t="s">
         <v>25</v>
       </c>
@@ -3501,7 +3532,7 @@
       <c r="O86" s="4"/>
     </row>
     <row r="87" spans="2:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="L87" s="51"/>
+      <c r="L87" s="52"/>
       <c r="M87" s="5" t="s">
         <v>26</v>
       </c>
@@ -3510,7 +3541,7 @@
     </row>
     <row r="88" spans="2:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="89" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="L89" s="50" t="s">
+      <c r="L89" s="53" t="s">
         <v>99</v>
       </c>
       <c r="M89" s="12" t="s">
@@ -3520,7 +3551,7 @@
       <c r="O89" s="13"/>
     </row>
     <row r="90" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="L90" s="52"/>
+      <c r="L90" s="51"/>
       <c r="M90" s="3" t="s">
         <v>25</v>
       </c>
@@ -3528,11 +3559,11 @@
         <v>180</v>
       </c>
       <c r="O90" s="4" t="s">
-        <v>204</v>
+        <v>201</v>
       </c>
     </row>
     <row r="91" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="L91" s="53"/>
+      <c r="L91" s="54"/>
       <c r="M91" s="3" t="s">
         <v>26</v>
       </c>
@@ -3540,8 +3571,8 @@
       <c r="O91" s="4"/>
     </row>
     <row r="92" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="L92" s="54" t="s">
-        <v>203</v>
+      <c r="L92" s="50" t="s">
+        <v>200</v>
       </c>
       <c r="M92" s="3" t="s">
         <v>24</v>
@@ -3550,19 +3581,19 @@
       <c r="O92" s="4"/>
     </row>
     <row r="93" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="L93" s="52"/>
+      <c r="L93" s="51"/>
       <c r="M93" s="3" t="s">
         <v>25</v>
       </c>
       <c r="N93" s="3" t="s">
-        <v>205</v>
+        <v>202</v>
       </c>
       <c r="O93" s="4" t="s">
-        <v>206</v>
+        <v>203</v>
       </c>
     </row>
     <row r="94" spans="2:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="L94" s="51"/>
+      <c r="L94" s="52"/>
       <c r="M94" s="5" t="s">
         <v>26</v>
       </c>
@@ -3571,7 +3602,7 @@
     </row>
     <row r="95" spans="2:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="96" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="L96" s="50" t="s">
+      <c r="L96" s="53" t="s">
         <v>97</v>
       </c>
       <c r="M96" s="12" t="s">
@@ -3581,7 +3612,7 @@
       <c r="O96" s="13"/>
     </row>
     <row r="97" spans="12:15" x14ac:dyDescent="0.25">
-      <c r="L97" s="52"/>
+      <c r="L97" s="51"/>
       <c r="M97" s="3" t="s">
         <v>25</v>
       </c>
@@ -3589,7 +3620,7 @@
       <c r="O97" s="4"/>
     </row>
     <row r="98" spans="12:15" x14ac:dyDescent="0.25">
-      <c r="L98" s="53"/>
+      <c r="L98" s="54"/>
       <c r="M98" s="3" t="s">
         <v>26</v>
       </c>
@@ -3597,7 +3628,7 @@
       <c r="O98" s="4"/>
     </row>
     <row r="99" spans="12:15" x14ac:dyDescent="0.25">
-      <c r="L99" s="54" t="s">
+      <c r="L99" s="50" t="s">
         <v>98</v>
       </c>
       <c r="M99" s="3" t="s">
@@ -3607,7 +3638,7 @@
       <c r="O99" s="4"/>
     </row>
     <row r="100" spans="12:15" x14ac:dyDescent="0.25">
-      <c r="L100" s="52"/>
+      <c r="L100" s="51"/>
       <c r="M100" s="3" t="s">
         <v>25</v>
       </c>
@@ -3615,7 +3646,7 @@
       <c r="O100" s="4"/>
     </row>
     <row r="101" spans="12:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="L101" s="51"/>
+      <c r="L101" s="52"/>
       <c r="M101" s="5" t="s">
         <v>26</v>
       </c>
@@ -3624,21 +3655,44 @@
     </row>
   </sheetData>
   <mergeCells count="69">
-    <mergeCell ref="L50:L52"/>
-    <mergeCell ref="L54:L56"/>
-    <mergeCell ref="L57:L59"/>
-    <mergeCell ref="L60:L62"/>
-    <mergeCell ref="L85:L87"/>
-    <mergeCell ref="L68:L70"/>
-    <mergeCell ref="L71:L73"/>
-    <mergeCell ref="L75:L77"/>
-    <mergeCell ref="L78:L80"/>
-    <mergeCell ref="L65:L67"/>
-    <mergeCell ref="L89:L91"/>
-    <mergeCell ref="L92:L94"/>
-    <mergeCell ref="L96:L98"/>
-    <mergeCell ref="L82:L84"/>
-    <mergeCell ref="L99:L101"/>
+    <mergeCell ref="L19:L20"/>
+    <mergeCell ref="L15:L17"/>
+    <mergeCell ref="L47:L49"/>
+    <mergeCell ref="L31:L33"/>
+    <mergeCell ref="L37:L39"/>
+    <mergeCell ref="L43:L45"/>
+    <mergeCell ref="L34:L36"/>
+    <mergeCell ref="L40:L42"/>
+    <mergeCell ref="G59:G61"/>
+    <mergeCell ref="B79:B81"/>
+    <mergeCell ref="G49:G51"/>
+    <mergeCell ref="G52:G54"/>
+    <mergeCell ref="B76:B78"/>
+    <mergeCell ref="B54:B56"/>
+    <mergeCell ref="G56:G58"/>
+    <mergeCell ref="G42:G44"/>
+    <mergeCell ref="G46:G48"/>
+    <mergeCell ref="G38:G40"/>
+    <mergeCell ref="B34:B36"/>
+    <mergeCell ref="B44:B46"/>
+    <mergeCell ref="B37:B39"/>
+    <mergeCell ref="B41:B43"/>
+    <mergeCell ref="B82:B84"/>
+    <mergeCell ref="B67:B69"/>
+    <mergeCell ref="B70:B72"/>
+    <mergeCell ref="B73:B75"/>
+    <mergeCell ref="G15:G17"/>
+    <mergeCell ref="G19:G21"/>
+    <mergeCell ref="G22:G24"/>
+    <mergeCell ref="G25:G27"/>
+    <mergeCell ref="G28:G30"/>
+    <mergeCell ref="B57:B59"/>
+    <mergeCell ref="B60:B62"/>
+    <mergeCell ref="B63:B65"/>
+    <mergeCell ref="B47:B49"/>
+    <mergeCell ref="B50:B52"/>
+    <mergeCell ref="B24:B26"/>
+    <mergeCell ref="B28:B30"/>
     <mergeCell ref="B31:B33"/>
     <mergeCell ref="B18:B20"/>
     <mergeCell ref="B2:O2"/>
@@ -3655,44 +3709,21 @@
     <mergeCell ref="L7:L8"/>
     <mergeCell ref="L10:L11"/>
     <mergeCell ref="L13:L14"/>
-    <mergeCell ref="B82:B84"/>
-    <mergeCell ref="B67:B69"/>
-    <mergeCell ref="B70:B72"/>
-    <mergeCell ref="B73:B75"/>
-    <mergeCell ref="G15:G17"/>
-    <mergeCell ref="G19:G21"/>
-    <mergeCell ref="G22:G24"/>
-    <mergeCell ref="G25:G27"/>
-    <mergeCell ref="G28:G30"/>
-    <mergeCell ref="B57:B59"/>
-    <mergeCell ref="B60:B62"/>
-    <mergeCell ref="B63:B65"/>
-    <mergeCell ref="B47:B49"/>
-    <mergeCell ref="B50:B52"/>
-    <mergeCell ref="B24:B26"/>
-    <mergeCell ref="B28:B30"/>
-    <mergeCell ref="G42:G44"/>
-    <mergeCell ref="G46:G48"/>
-    <mergeCell ref="G38:G40"/>
-    <mergeCell ref="B34:B36"/>
-    <mergeCell ref="B44:B46"/>
-    <mergeCell ref="B37:B39"/>
-    <mergeCell ref="B41:B43"/>
-    <mergeCell ref="G59:G61"/>
-    <mergeCell ref="B79:B81"/>
-    <mergeCell ref="G49:G51"/>
-    <mergeCell ref="G52:G54"/>
-    <mergeCell ref="B76:B78"/>
-    <mergeCell ref="B54:B56"/>
-    <mergeCell ref="G56:G58"/>
-    <mergeCell ref="L19:L20"/>
-    <mergeCell ref="L15:L17"/>
-    <mergeCell ref="L47:L49"/>
-    <mergeCell ref="L31:L33"/>
-    <mergeCell ref="L37:L39"/>
-    <mergeCell ref="L43:L45"/>
-    <mergeCell ref="L34:L36"/>
-    <mergeCell ref="L40:L42"/>
+    <mergeCell ref="L89:L91"/>
+    <mergeCell ref="L92:L94"/>
+    <mergeCell ref="L96:L98"/>
+    <mergeCell ref="L82:L84"/>
+    <mergeCell ref="L99:L101"/>
+    <mergeCell ref="L50:L52"/>
+    <mergeCell ref="L54:L56"/>
+    <mergeCell ref="L57:L59"/>
+    <mergeCell ref="L60:L62"/>
+    <mergeCell ref="L85:L87"/>
+    <mergeCell ref="L68:L70"/>
+    <mergeCell ref="L71:L73"/>
+    <mergeCell ref="L75:L77"/>
+    <mergeCell ref="L78:L80"/>
+    <mergeCell ref="L65:L67"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" scale="44" orientation="portrait" r:id="rId1"/>

</xml_diff>